<commit_message>
Removed Unused code chase
</commit_message>
<xml_diff>
--- a/Scheduling/Schedule/Schedule-Team4 (2).xlsx
+++ b/Scheduling/Schedule/Schedule-Team4 (2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\School Account\Desktop\Team4Project\Scheduling\Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FBBB55-79C5-490F-9D83-744CA883DDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C74F252-E258-46DE-81C4-302C41AD5673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="317">
   <si>
     <t>Task#</t>
   </si>
@@ -987,6 +987,12 @@
   </si>
   <si>
     <t>3 Hour</t>
+  </si>
+  <si>
+    <t>2 Hours</t>
+  </si>
+  <si>
+    <t>1 Hour</t>
   </si>
 </sst>
 </file>
@@ -3521,7 +3527,7 @@
   <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="L110" sqref="L110"/>
+      <selection activeCell="M115" sqref="M115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7612,8 +7618,8 @@
       <c r="B110" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="L110" s="19">
-        <v>2</v>
+      <c r="L110" s="19" t="s">
+        <v>315</v>
       </c>
       <c r="M110" s="19" t="s">
         <v>37</v>
@@ -7635,19 +7641,31 @@
         <v>310</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="L113" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="M113" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
         <v>313</v>
+      </c>
+      <c r="L115" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="M115" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>